<commit_message>
Lates with multiple changes
</commit_message>
<xml_diff>
--- a/Data Extraction And Loading/Program Files/Documentation/Imported Data Summary.xlsx
+++ b/Data Extraction And Loading/Program Files/Documentation/Imported Data Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuck\Documents\ROC\Speedway-Source\Data Extraction And Loading\Program Files\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFC2F69-C186-4555-B592-C93097C39E27}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111471BE-193E-4947-B8CC-DE03885F12B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21900" windowHeight="6705" xr2:uid="{35CC5D13-6FA0-4E86-8B8E-1E92ADCCBFD3}"/>
+    <workbookView xWindow="1440" yWindow="1308" windowWidth="21600" windowHeight="11652" xr2:uid="{35CC5D13-6FA0-4E86-8B8E-1E92ADCCBFD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Imported Data" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="57">
   <si>
     <t>Item Hierarchy</t>
   </si>
@@ -98,9 +98,6 @@
     <t>50 Groups per batch</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>Business_Unit_Group_X (X=Batch Number)</t>
   </si>
   <si>
@@ -180,6 +177,30 @@
   </si>
   <si>
     <t>1 file per special.</t>
+  </si>
+  <si>
+    <t>No longer used</t>
+  </si>
+  <si>
+    <t>Fuel Tank Types</t>
+  </si>
+  <si>
+    <t>Fuel Tanks</t>
+  </si>
+  <si>
+    <t>approx 200</t>
+  </si>
+  <si>
+    <t>approx 500</t>
+  </si>
+  <si>
+    <t>approx 1800</t>
+  </si>
+  <si>
+    <t>Approx 50</t>
+  </si>
+  <si>
+    <t>Approx 80</t>
   </si>
 </sst>
 </file>
@@ -601,24 +622,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4CB35B-6870-433F-A7B5-B455E6ED0866}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="14" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="14" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -644,7 +665,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -664,9 +685,11 @@
         <v>9</v>
       </c>
       <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="H2" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -674,31 +697,31 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>19</v>
@@ -710,9 +733,11 @@
         <v>9</v>
       </c>
       <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H4" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -720,7 +745,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>19</v>
@@ -734,12 +759,12 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="8" t="s">
@@ -750,12 +775,12 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="8" t="s">
@@ -766,36 +791,36 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="3">
-        <v>60</v>
+      <c r="E8" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="8" t="s">
@@ -806,18 +831,18 @@
       <c r="G9" s="9"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -828,7 +853,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>4</v>
       </c>
@@ -836,7 +861,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>19</v>
@@ -850,15 +875,15 @@
       <c r="G11" s="6"/>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>19</v>
@@ -872,15 +897,15 @@
       <c r="G12" s="6"/>
       <c r="H12" s="12"/>
     </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>19</v>
@@ -894,21 +919,21 @@
       <c r="G13" s="6"/>
       <c r="H13" s="12"/>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="D14" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="7">
-        <v>1777</v>
+        <v>42</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>8</v>
@@ -916,12 +941,12 @@
       <c r="G14" s="6"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8" t="s">
@@ -930,47 +955,80 @@
       <c r="E15" s="7"/>
       <c r="F15" s="11"/>
     </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="8" t="s">
+      <c r="D16" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="E16" s="10" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>